<commit_message>
in need some UI
</commit_message>
<xml_diff>
--- a/assets/files/name.xlsx
+++ b/assets/files/name.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\Desktop\Flutter_Project\testttttttttttt\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>yamen</t>
-  </si>
-  <si>
-    <t>محمد نديم الحلاق</t>
+    <t>انما الاعمال بالنيات وانما لكل امرئ ما نوى فمن كانت هجرته الى الله و رسوله فهجرته الى الله و رسوله و من كانت هجرته لدنيا يصيبها او امراه ينكحها فهجرته الى ما هاجر اليه</t>
   </si>
 </sst>
 </file>
@@ -340,34 +337,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="93" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>